<commit_message>
add part II data pre-processing
</commit_message>
<xml_diff>
--- a/Analyses/part_II/outputs/01_dataPreperation/final/networkIndicators.xlsx
+++ b/Analyses/part_II/outputs/01_dataPreperation/final/networkIndicators.xlsx
@@ -1873,7 +1873,7 @@
         <v>0.5284148185483871</v>
       </c>
       <c r="K2" t="n">
-        <v>0.8323356583550784</v>
+        <v>0.8323356583550783</v>
       </c>
       <c r="L2" t="n">
         <v>4.494318181818182</v>
@@ -2259,7 +2259,7 @@
         <v>0.8099798387096774</v>
       </c>
       <c r="K3" t="n">
-        <v>0.8102552671850957</v>
+        <v>0.8102552671850956</v>
       </c>
       <c r="L3" t="n">
         <v>3.9583333333333335</v>
@@ -2645,7 +2645,7 @@
         <v>0.7778477822580645</v>
       </c>
       <c r="K4" t="n">
-        <v>0.8075815857467289</v>
+        <v>0.8075815857467287</v>
       </c>
       <c r="L4" t="n">
         <v>2.992424242424242</v>
@@ -3031,7 +3031,7 @@
         <v>0.7057081653225806</v>
       </c>
       <c r="K5" t="n">
-        <v>0.7535271802753924</v>
+        <v>0.7535271802753927</v>
       </c>
       <c r="L5" t="n">
         <v>5.962121212121212</v>
@@ -4189,7 +4189,7 @@
         <v>0.3561964465725807</v>
       </c>
       <c r="K8" t="n">
-        <v>0.6942552739016337</v>
+        <v>0.6942552739016336</v>
       </c>
       <c r="L8" t="n">
         <v>5.994318181818182</v>
@@ -4575,7 +4575,7 @@
         <v>0.4064390120967742</v>
       </c>
       <c r="K9" t="n">
-        <v>0.688346458372564</v>
+        <v>0.6883464583725638</v>
       </c>
       <c r="L9" t="n">
         <v>5.045454545454546</v>
@@ -4961,7 +4961,7 @@
         <v>0.7838961693548387</v>
       </c>
       <c r="K10" t="n">
-        <v>0.78787825088942</v>
+        <v>0.7878782508894198</v>
       </c>
       <c r="L10" t="n">
         <v>4.5606060606060606</v>
@@ -5347,7 +5347,7 @@
         <v>0.27301447292626724</v>
       </c>
       <c r="K11" t="n">
-        <v>0.7269938336405788</v>
+        <v>0.7269938336405793</v>
       </c>
       <c r="L11" t="n">
         <v>3.9943181818181817</v>
@@ -5733,7 +5733,7 @@
         <v>0.7809979838709679</v>
       </c>
       <c r="K12" t="n">
-        <v>0.8193855942862852</v>
+        <v>0.8193855942862854</v>
       </c>
       <c r="L12" t="n">
         <v>2.7481060606060606</v>
@@ -6891,7 +6891,7 @@
         <v>0.6046496975806451</v>
       </c>
       <c r="K15" t="n">
-        <v>0.8048101383672205</v>
+        <v>0.8048101383672207</v>
       </c>
       <c r="L15" t="n">
         <v>7.257575757575758</v>
@@ -7277,7 +7277,7 @@
         <v>0.5996633784562212</v>
       </c>
       <c r="K16" t="n">
-        <v>0.7983577904246384</v>
+        <v>0.7983577904246386</v>
       </c>
       <c r="L16" t="n">
         <v>4.708333333333333</v>
@@ -8049,7 +8049,7 @@
         <v>0.39342147654534904</v>
       </c>
       <c r="K18" t="n">
-        <v>0.6486522940218341</v>
+        <v>0.6486522940218342</v>
       </c>
       <c r="L18" t="n">
         <v>3.0492424242424243</v>
@@ -8821,7 +8821,7 @@
         <v>0.5760296658986176</v>
       </c>
       <c r="K20" t="n">
-        <v>0.8037068744491485</v>
+        <v>0.8037068744491482</v>
       </c>
       <c r="L20" t="n">
         <v>6.6647727272727275</v>
@@ -9207,7 +9207,7 @@
         <v>0.7754536290322581</v>
       </c>
       <c r="K21" t="n">
-        <v>0.8182420876700931</v>
+        <v>0.8182420876700928</v>
       </c>
       <c r="L21" t="n">
         <v>7.537878787878788</v>
@@ -10751,7 +10751,7 @@
         <v>0.7448336693548387</v>
       </c>
       <c r="K25" t="n">
-        <v>0.7163428837254009</v>
+        <v>0.7163428837254006</v>
       </c>
       <c r="L25" t="n">
         <v>4.670454545454546</v>
@@ -11137,7 +11137,7 @@
         <v>0.9253402217741935</v>
       </c>
       <c r="K26" t="n">
-        <v>0.8653709817025532</v>
+        <v>0.865370981702553</v>
       </c>
       <c r="L26" t="n">
         <v>2.804924242424242</v>
@@ -11523,7 +11523,7 @@
         <v>0.5613659274193549</v>
       </c>
       <c r="K27" t="n">
-        <v>0.7932281696726766</v>
+        <v>0.7932281696726772</v>
       </c>
       <c r="L27" t="n">
         <v>6.170454545454546</v>
@@ -11909,7 +11909,7 @@
         <v>0.7960559475806451</v>
       </c>
       <c r="K28" t="n">
-        <v>0.8309971733063409</v>
+        <v>0.8309971733063414</v>
       </c>
       <c r="L28" t="n">
         <v>2.8863636363636362</v>
@@ -13065,7 +13065,7 @@
         <v>0.49489667338709675</v>
       </c>
       <c r="K31" t="n">
-        <v>0.8197643151939793</v>
+        <v>0.8197643151939789</v>
       </c>
       <c r="L31" t="n">
         <v>4.9356060606060606</v>
@@ -13451,7 +13451,7 @@
         <v>0.22501073145604392</v>
       </c>
       <c r="K32" t="n">
-        <v>0.6285398419785793</v>
+        <v>0.6285398419785786</v>
       </c>
       <c r="L32" t="n">
         <v>3.8882575757575757</v>
@@ -13837,7 +13837,7 @@
         <v>0.8228326612903226</v>
       </c>
       <c r="K33" t="n">
-        <v>0.8679119545566171</v>
+        <v>0.8679119545566173</v>
       </c>
       <c r="L33" t="n">
         <v>3.6363636363636362</v>
@@ -14609,7 +14609,7 @@
         <v>0.577179939516129</v>
       </c>
       <c r="K35" t="n">
-        <v>0.8311784046795545</v>
+        <v>0.8311784046795542</v>
       </c>
       <c r="L35" t="n">
         <v>4.683712121212121</v>
@@ -14995,7 +14995,7 @@
         <v>0.5210748487903226</v>
       </c>
       <c r="K36" t="n">
-        <v>0.8175437586302488</v>
+        <v>0.8175437586302486</v>
       </c>
       <c r="L36" t="n">
         <v>5.59280303030303</v>
@@ -15381,7 +15381,7 @@
         <v>0.5831338205645161</v>
       </c>
       <c r="K37" t="n">
-        <v>0.6929702312693622</v>
+        <v>0.6929702312693616</v>
       </c>
       <c r="L37" t="n">
         <v>6.257575757575758</v>
@@ -16153,7 +16153,7 @@
         <v>0.7035696284562213</v>
       </c>
       <c r="K39" t="n">
-        <v>0.8449363289191932</v>
+        <v>0.844936328919193</v>
       </c>
       <c r="L39" t="n">
         <v>6.628787878787879</v>
@@ -16539,7 +16539,7 @@
         <v>0.3048450100806452</v>
       </c>
       <c r="K40" t="n">
-        <v>0.7818121094745386</v>
+        <v>0.7818121094745388</v>
       </c>
       <c r="L40" t="n">
         <v>4.488636363636363</v>
@@ -16925,7 +16925,7 @@
         <v>0.6334425403225806</v>
       </c>
       <c r="K41" t="n">
-        <v>0.7747759258224265</v>
+        <v>0.7747759258224263</v>
       </c>
       <c r="L41" t="n">
         <v>3.5625</v>
@@ -17311,7 +17311,7 @@
         <v>0.4610635080645161</v>
       </c>
       <c r="K42" t="n">
-        <v>0.7877508463953022</v>
+        <v>0.787750846395303</v>
       </c>
       <c r="L42" t="n">
         <v>8.482954545454545</v>
@@ -17697,7 +17697,7 @@
         <v>0.6262474798387098</v>
       </c>
       <c r="K43" t="n">
-        <v>0.8028117312062165</v>
+        <v>0.8028117312062167</v>
       </c>
       <c r="L43" t="n">
         <v>3.1571969696969697</v>
@@ -18083,7 +18083,7 @@
         <v>0.6295992943548387</v>
       </c>
       <c r="K44" t="n">
-        <v>0.8133185404162526</v>
+        <v>0.8133185404162531</v>
       </c>
       <c r="L44" t="n">
         <v>9.571969696969697</v>
@@ -18469,7 +18469,7 @@
         <v>0.3424944196428571</v>
       </c>
       <c r="K45" t="n">
-        <v>0.7090931053457291</v>
+        <v>0.709093105345729</v>
       </c>
       <c r="L45" t="n">
         <v>4.15530303030303</v>
@@ -20013,7 +20013,7 @@
         <v>0.6103515625</v>
       </c>
       <c r="K49" t="n">
-        <v>0.8018923215247439</v>
+        <v>0.8018923215247434</v>
       </c>
       <c r="L49" t="n">
         <v>4.958333333333333</v>
@@ -20785,7 +20785,7 @@
         <v>0.6125702044930875</v>
       </c>
       <c r="K51" t="n">
-        <v>0.7225710144665956</v>
+        <v>0.7225710144665961</v>
       </c>
       <c r="L51" t="n">
         <v>2.672348484848485</v>
@@ -21557,7 +21557,7 @@
         <v>0.41655115927419356</v>
       </c>
       <c r="K53" t="n">
-        <v>0.7819998392808721</v>
+        <v>0.7819998392808725</v>
       </c>
       <c r="L53" t="n">
         <v>7.153409090909091</v>
@@ -21943,7 +21943,7 @@
         <v>0.6133442540322581</v>
       </c>
       <c r="K54" t="n">
-        <v>0.8233208749722818</v>
+        <v>0.8233208749722816</v>
       </c>
       <c r="L54" t="n">
         <v>5.428030303030303</v>
@@ -23487,7 +23487,7 @@
         <v>0.810704385080645</v>
       </c>
       <c r="K58" t="n">
-        <v>0.8100410963246133</v>
+        <v>0.8100410963246136</v>
       </c>
       <c r="L58" t="n">
         <v>3.7045454545454546</v>
@@ -23873,7 +23873,7 @@
         <v>0.6790574596774194</v>
       </c>
       <c r="K59" t="n">
-        <v>0.8539608046721276</v>
+        <v>0.8539608046721271</v>
       </c>
       <c r="L59" t="n">
         <v>5.619318181818182</v>
@@ -25031,7 +25031,7 @@
         <v>0.606413810483871</v>
       </c>
       <c r="K62" t="n">
-        <v>0.6909438795984532</v>
+        <v>0.6909438795984529</v>
       </c>
       <c r="L62" t="n">
         <v>6.511363636363637</v>
@@ -25417,7 +25417,7 @@
         <v>0.6164944556451613</v>
       </c>
       <c r="K63" t="n">
-        <v>0.8078657042322901</v>
+        <v>0.8078657042322905</v>
       </c>
       <c r="L63" t="n">
         <v>4.3143939393939394</v>
@@ -25803,7 +25803,7 @@
         <v>0.8315902217741935</v>
       </c>
       <c r="K64" t="n">
-        <v>0.8589271996333092</v>
+        <v>0.8589271996333093</v>
       </c>
       <c r="L64" t="n">
         <v>5.073863636363637</v>
@@ -26189,7 +26189,7 @@
         <v>0.4772051411290323</v>
       </c>
       <c r="K65" t="n">
-        <v>0.7529784929913091</v>
+        <v>0.7529784929913093</v>
       </c>
       <c r="L65" t="n">
         <v>5.604166666666667</v>
@@ -27347,7 +27347,7 @@
         <v>0.6887915826612904</v>
       </c>
       <c r="K68" t="n">
-        <v>0.743185312294892</v>
+        <v>0.7431853122948924</v>
       </c>
       <c r="L68" t="n">
         <v>4.100378787878788</v>
@@ -29663,7 +29663,7 @@
         <v>0.9017137096774194</v>
       </c>
       <c r="K74" t="n">
-        <v>0.8534602167155368</v>
+        <v>0.8534602167155371</v>
       </c>
       <c r="L74" t="n">
         <v>3.2386363636363638</v>
@@ -30049,7 +30049,7 @@
         <v>0.7670740927419355</v>
       </c>
       <c r="K75" t="n">
-        <v>0.7896436394706853</v>
+        <v>0.789643639470685</v>
       </c>
       <c r="L75" t="n">
         <v>6.859848484848484</v>
@@ -30435,7 +30435,7 @@
         <v>0.6422631048387094</v>
       </c>
       <c r="K76" t="n">
-        <v>0.7545667148537128</v>
+        <v>0.754566714853713</v>
       </c>
       <c r="L76" t="n">
         <v>5.191287878787879</v>
@@ -30821,7 +30821,7 @@
         <v>0.8162802419354839</v>
       </c>
       <c r="K77" t="n">
-        <v>0.8412926058869493</v>
+        <v>0.8412926058869492</v>
       </c>
       <c r="L77" t="n">
         <v>5.6647727272727275</v>
@@ -31207,7 +31207,7 @@
         <v>0.9691595262096774</v>
       </c>
       <c r="K78" t="n">
-        <v>0.8490966083419491</v>
+        <v>0.849096608341949</v>
       </c>
       <c r="L78" t="n">
         <v>3.4393939393939394</v>
@@ -31979,7 +31979,7 @@
         <v>0.582019999279954</v>
       </c>
       <c r="K80" t="n">
-        <v>0.7596217990213584</v>
+        <v>0.7596217990213586</v>
       </c>
       <c r="L80" t="n">
         <v>6.028409090909091</v>
@@ -32365,7 +32365,7 @@
         <v>0.9017137096774194</v>
       </c>
       <c r="K81" t="n">
-        <v>0.8631353493220087</v>
+        <v>0.8631353493220089</v>
       </c>
       <c r="L81" t="n">
         <v>3.6609848484848486</v>
@@ -32751,7 +32751,7 @@
         <v>0.8627362651209676</v>
       </c>
       <c r="K82" t="n">
-        <v>0.8078169042803328</v>
+        <v>0.8078169042803331</v>
       </c>
       <c r="L82" t="n">
         <v>2.375</v>
@@ -33137,7 +33137,7 @@
         <v>0.8761025705645161</v>
       </c>
       <c r="K83" t="n">
-        <v>0.8499049362878651</v>
+        <v>0.849904936287865</v>
       </c>
       <c r="L83" t="n">
         <v>4.34280303030303</v>
@@ -33523,7 +33523,7 @@
         <v>0.7202620967741935</v>
       </c>
       <c r="K84" t="n">
-        <v>0.7431682322065604</v>
+        <v>0.7431682322065607</v>
       </c>
       <c r="L84" t="n">
         <v>3.4109848484848486</v>
@@ -36225,7 +36225,7 @@
         <v>0.8319682459677419</v>
       </c>
       <c r="K91" t="n">
-        <v>0.866600410710564</v>
+        <v>0.8666004107105639</v>
       </c>
       <c r="L91" t="n">
         <v>5.8977272727272725</v>
@@ -36611,7 +36611,7 @@
         <v>0.7638608870967742</v>
       </c>
       <c r="K92" t="n">
-        <v>0.8580253023314183</v>
+        <v>0.858025302331418</v>
       </c>
       <c r="L92" t="n">
         <v>4.863636363636363</v>
@@ -37383,7 +37383,7 @@
         <v>0.3296055947580645</v>
       </c>
       <c r="K94" t="n">
-        <v>0.8034856551969781</v>
+        <v>0.8034856551969782</v>
       </c>
       <c r="L94" t="n">
         <v>6.568181818181818</v>
@@ -37769,7 +37769,7 @@
         <v>0.8097908266129032</v>
       </c>
       <c r="K95" t="n">
-        <v>0.831228582117838</v>
+        <v>0.8312285821178382</v>
       </c>
       <c r="L95" t="n">
         <v>4.267045454545454</v>
@@ -38539,7 +38539,7 @@
         <v>0.6746471774193549</v>
       </c>
       <c r="K97" t="n">
-        <v>0.7763923695873178</v>
+        <v>0.7763923695873175</v>
       </c>
       <c r="L97" t="n">
         <v>6.9602272727272725</v>
@@ -38925,7 +38925,7 @@
         <v>0.2710361463133641</v>
       </c>
       <c r="K98" t="n">
-        <v>0.7317497810761585</v>
+        <v>0.7317497810761586</v>
       </c>
       <c r="L98" t="n">
         <v>5.4393939393939394</v>
@@ -40083,7 +40083,7 @@
         <v>0.6209992439516129</v>
       </c>
       <c r="K101" t="n">
-        <v>0.8276978894895275</v>
+        <v>0.8276978894895277</v>
       </c>
       <c r="L101" t="n">
         <v>5.456439393939394</v>
@@ -40469,7 +40469,7 @@
         <v>0.7983803463421659</v>
       </c>
       <c r="K102" t="n">
-        <v>0.8168864014052083</v>
+        <v>0.8168864014052085</v>
       </c>
       <c r="L102" t="n">
         <v>4.678030303030303</v>
@@ -40855,7 +40855,7 @@
         <v>0.6517137096774194</v>
       </c>
       <c r="K103" t="n">
-        <v>0.7511597364880744</v>
+        <v>0.7511597364880745</v>
       </c>
       <c r="L103" t="n">
         <v>4.138257575757576</v>
@@ -41241,7 +41241,7 @@
         <v>0.6651335685483871</v>
       </c>
       <c r="K104" t="n">
-        <v>0.836742192102181</v>
+        <v>0.8367421921021808</v>
       </c>
       <c r="L104" t="n">
         <v>5.8106060606060606</v>
@@ -41627,7 +41627,7 @@
         <v>0.5372983870967742</v>
       </c>
       <c r="K105" t="n">
-        <v>0.8754612729518696</v>
+        <v>0.8754612729518683</v>
       </c>
       <c r="L105" t="n">
         <v>7.9602272727272725</v>
@@ -42013,7 +42013,7 @@
         <v>0.6549899193548387</v>
       </c>
       <c r="K106" t="n">
-        <v>0.8052424027497251</v>
+        <v>0.8052424027497254</v>
       </c>
       <c r="L106" t="n">
         <v>6.660984848484849</v>
@@ -42785,7 +42785,7 @@
         <v>0.8844506048387096</v>
       </c>
       <c r="K108" t="n">
-        <v>0.8688357659325943</v>
+        <v>0.8688357659325944</v>
       </c>
       <c r="L108" t="n">
         <v>3.831439393939394</v>
@@ -43943,7 +43943,7 @@
         <v>0.4497992871543779</v>
       </c>
       <c r="K111" t="n">
-        <v>0.7572925867229483</v>
+        <v>0.7572925867229479</v>
       </c>
       <c r="L111" t="n">
         <v>3.9981060606060606</v>
@@ -44329,7 +44329,7 @@
         <v>0.8748739919354839</v>
       </c>
       <c r="K112" t="n">
-        <v>0.8676511162889617</v>
+        <v>0.8676511162889619</v>
       </c>
       <c r="L112" t="n">
         <v>3.191287878787879</v>
@@ -44715,7 +44715,7 @@
         <v>0.9147555443548387</v>
       </c>
       <c r="K113" t="n">
-        <v>0.8544534169445295</v>
+        <v>0.8544534169445299</v>
       </c>
       <c r="L113" t="n">
         <v>2.6931818181818183</v>
@@ -45101,7 +45101,7 @@
         <v>0.7692162298387096</v>
       </c>
       <c r="K114" t="n">
-        <v>0.8740027259631371</v>
+        <v>0.8740027259631372</v>
       </c>
       <c r="L114" t="n">
         <v>8.0</v>
@@ -45487,7 +45487,7 @@
         <v>0.6410975302419355</v>
       </c>
       <c r="K115" t="n">
-        <v>0.8228232760497195</v>
+        <v>0.82282327604972</v>
       </c>
       <c r="L115" t="n">
         <v>4.083333333333333</v>
@@ -45873,7 +45873,7 @@
         <v>0.6438382056451613</v>
       </c>
       <c r="K116" t="n">
-        <v>0.8564304711651703</v>
+        <v>0.8564304711651702</v>
       </c>
       <c r="L116" t="n">
         <v>4.893939393939394</v>
@@ -46259,7 +46259,7 @@
         <v>0.584078881048387</v>
       </c>
       <c r="K117" t="n">
-        <v>0.8134885504190347</v>
+        <v>0.8134885504190349</v>
       </c>
       <c r="L117" t="n">
         <v>5.409090909090909</v>
@@ -47031,7 +47031,7 @@
         <v>0.4065020161290322</v>
       </c>
       <c r="K119" t="n">
-        <v>0.7335913806075022</v>
+        <v>0.7335913806075024</v>
       </c>
       <c r="L119" t="n">
         <v>5.918560606060606</v>
@@ -47417,7 +47417,7 @@
         <v>0.5822202620967742</v>
       </c>
       <c r="K120" t="n">
-        <v>0.7962268961690856</v>
+        <v>0.7962268961690852</v>
       </c>
       <c r="L120" t="n">
         <v>5.992424242424242</v>
@@ -48189,7 +48189,7 @@
         <v>0.55859375</v>
       </c>
       <c r="K122" t="n">
-        <v>0.807412006655622</v>
+        <v>0.8074120066556219</v>
       </c>
       <c r="L122" t="n">
         <v>5.653409090909091</v>
@@ -50119,7 +50119,7 @@
         <v>0.8483492943548387</v>
       </c>
       <c r="K127" t="n">
-        <v>0.845808426932477</v>
+        <v>0.8458084269324772</v>
       </c>
       <c r="L127" t="n">
         <v>2.5890151515151514</v>
@@ -50891,7 +50891,7 @@
         <v>0.3480027721774194</v>
       </c>
       <c r="K129" t="n">
-        <v>0.8103284661560654</v>
+        <v>0.8103284661560655</v>
       </c>
       <c r="L129" t="n">
         <v>3.587121212121212</v>
@@ -51277,7 +51277,7 @@
         <v>0.3945661791585431</v>
       </c>
       <c r="K130" t="n">
-        <v>0.6721441424803858</v>
+        <v>0.6721441424803853</v>
       </c>
       <c r="L130" t="n">
         <v>3.6458333333333335</v>
@@ -51663,7 +51663,7 @@
         <v>0.6544273833525345</v>
       </c>
       <c r="K131" t="n">
-        <v>0.7578249292936556</v>
+        <v>0.7578249292936557</v>
       </c>
       <c r="L131" t="n">
         <v>5.446969696969697</v>
@@ -52049,7 +52049,7 @@
         <v>0.6796938004032257</v>
       </c>
       <c r="K132" t="n">
-        <v>0.8153002813950428</v>
+        <v>0.8153002813950431</v>
       </c>
       <c r="L132" t="n">
         <v>4.537878787878788</v>
@@ -52435,7 +52435,7 @@
         <v>0.6535408266129032</v>
       </c>
       <c r="K133" t="n">
-        <v>0.796622965753092</v>
+        <v>0.7966229657530922</v>
       </c>
       <c r="L133" t="n">
         <v>3.7007575757575757</v>
@@ -52821,7 +52821,7 @@
         <v>0.6506426411290323</v>
       </c>
       <c r="K134" t="n">
-        <v>0.7904911003566503</v>
+        <v>0.79049110035665</v>
       </c>
       <c r="L134" t="n">
         <v>5.471590909090909</v>
@@ -53207,7 +53207,7 @@
         <v>0.4867376512096773</v>
       </c>
       <c r="K135" t="n">
-        <v>0.7464856608242139</v>
+        <v>0.7464856608242141</v>
       </c>
       <c r="L135" t="n">
         <v>5.024621212121212</v>
@@ -53593,7 +53593,7 @@
         <v>0.9497227822580645</v>
       </c>
       <c r="K136" t="n">
-        <v>0.8383723968710558</v>
+        <v>0.8383723968710556</v>
       </c>
       <c r="L136" t="n">
         <v>3.242424242424242</v>
@@ -54365,7 +54365,7 @@
         <v>0.18033329133064505</v>
       </c>
       <c r="K138" t="n">
-        <v>0.7392205254486423</v>
+        <v>0.739220525448642</v>
       </c>
       <c r="L138" t="n">
         <v>3.865530303030303</v>
@@ -55137,7 +55137,7 @@
         <v>0.2897427935387865</v>
       </c>
       <c r="K140" t="n">
-        <v>0.6853080941788459</v>
+        <v>0.6853080941788458</v>
       </c>
       <c r="L140" t="n">
         <v>2.7765151515151514</v>
@@ -55909,7 +55909,7 @@
         <v>0.4490297379032258</v>
       </c>
       <c r="K142" t="n">
-        <v>0.6975678400250122</v>
+        <v>0.6975678400250124</v>
       </c>
       <c r="L142" t="n">
         <v>4.863636363636363</v>
@@ -56295,7 +56295,7 @@
         <v>0.4747983870967742</v>
       </c>
       <c r="K143" t="n">
-        <v>0.8293317176416007</v>
+        <v>0.8293317176416011</v>
       </c>
       <c r="L143" t="n">
         <v>6.4772727272727275</v>
@@ -56681,7 +56681,7 @@
         <v>0.6290322580645161</v>
       </c>
       <c r="K144" t="n">
-        <v>0.7684703325448894</v>
+        <v>0.7684703325448895</v>
       </c>
       <c r="L144" t="n">
         <v>3.0359848484848486</v>
@@ -57067,7 +57067,7 @@
         <v>0.7146547379032258</v>
       </c>
       <c r="K145" t="n">
-        <v>0.8573817277625267</v>
+        <v>0.8573817277625272</v>
       </c>
       <c r="L145" t="n">
         <v>6.583333333333333</v>
@@ -57839,7 +57839,7 @@
         <v>0.8445060483870968</v>
       </c>
       <c r="K147" t="n">
-        <v>0.8400140686227194</v>
+        <v>0.8400140686227197</v>
       </c>
       <c r="L147" t="n">
         <v>4.636363636363637</v>
@@ -58225,7 +58225,7 @@
         <v>0.6004284274193549</v>
       </c>
       <c r="K148" t="n">
-        <v>0.8089751201889519</v>
+        <v>0.8089751201889522</v>
       </c>
       <c r="L148" t="n">
         <v>4.071969696969697</v>
@@ -59383,7 +59383,7 @@
         <v>0.7212071572580645</v>
       </c>
       <c r="K151" t="n">
-        <v>0.8298144802682011</v>
+        <v>0.8298144802682014</v>
       </c>
       <c r="L151" t="n">
         <v>4.8768939393939394</v>
@@ -59769,7 +59769,7 @@
         <v>0.9214339717741935</v>
       </c>
       <c r="K152" t="n">
-        <v>0.8559951932723785</v>
+        <v>0.8559951932723784</v>
       </c>
       <c r="L152" t="n">
         <v>3.6761363636363638</v>
@@ -60155,7 +60155,7 @@
         <v>0.668913810483871</v>
       </c>
       <c r="K153" t="n">
-        <v>0.7947715075325381</v>
+        <v>0.7947715075325379</v>
       </c>
       <c r="L153" t="n">
         <v>4.729166666666667</v>
@@ -60541,7 +60541,7 @@
         <v>0.67578125</v>
       </c>
       <c r="K154" t="n">
-        <v>0.799335789925329</v>
+        <v>0.7993357899253288</v>
       </c>
       <c r="L154" t="n">
         <v>5.3106060606060606</v>
@@ -60927,7 +60927,7 @@
         <v>0.7098664314516129</v>
       </c>
       <c r="K155" t="n">
-        <v>0.8294396717988664</v>
+        <v>0.8294396717988662</v>
       </c>
       <c r="L155" t="n">
         <v>5.6893939393939394</v>
@@ -61313,7 +61313,7 @@
         <v>0.5257056451612904</v>
       </c>
       <c r="K156" t="n">
-        <v>0.8047152598221585</v>
+        <v>0.8047152598221571</v>
       </c>
       <c r="L156" t="n">
         <v>6.5227272727272725</v>
@@ -62085,7 +62085,7 @@
         <v>0.8764805947580645</v>
       </c>
       <c r="K158" t="n">
-        <v>0.8290222301400147</v>
+        <v>0.8290222301400149</v>
       </c>
       <c r="L158" t="n">
         <v>3.6193181818181817</v>
@@ -62471,7 +62471,7 @@
         <v>0.8270539314516129</v>
       </c>
       <c r="K159" t="n">
-        <v>0.8220735689361567</v>
+        <v>0.8220735689361566</v>
       </c>
       <c r="L159" t="n">
         <v>3.210227272727273</v>
@@ -62857,7 +62857,7 @@
         <v>0.8296370967741935</v>
       </c>
       <c r="K160" t="n">
-        <v>0.8444704724311597</v>
+        <v>0.8444704724311596</v>
       </c>
       <c r="L160" t="n">
         <v>3.524621212121212</v>
@@ -63243,7 +63243,7 @@
         <v>0.6768523185483871</v>
       </c>
       <c r="K161" t="n">
-        <v>0.7092537095856136</v>
+        <v>0.7092537095856127</v>
       </c>
       <c r="L161" t="n">
         <v>8.149621212121213</v>
@@ -64015,7 +64015,7 @@
         <v>0.9212449596774194</v>
       </c>
       <c r="K163" t="n">
-        <v>0.8698609482325026</v>
+        <v>0.8698609482325025</v>
       </c>
       <c r="L163" t="n">
         <v>4.621212121212121</v>
@@ -64401,7 +64401,7 @@
         <v>0.23433792455024816</v>
       </c>
       <c r="K164" t="n">
-        <v>0.7922749207366363</v>
+        <v>0.7922749207366364</v>
       </c>
       <c r="L164" t="n">
         <v>5.848484848484849</v>
@@ -64787,7 +64787,7 @@
         <v>0.8187373991935484</v>
       </c>
       <c r="K165" t="n">
-        <v>0.8514246935798719</v>
+        <v>0.8514246935798718</v>
       </c>
       <c r="L165" t="n">
         <v>4.71780303030303</v>
@@ -65559,7 +65559,7 @@
         <v>0.6444682459677419</v>
       </c>
       <c r="K167" t="n">
-        <v>0.7421069157523801</v>
+        <v>0.7421069157523803</v>
       </c>
       <c r="L167" t="n">
         <v>5.125</v>
@@ -65945,7 +65945,7 @@
         <v>0.7355405745967742</v>
       </c>
       <c r="K168" t="n">
-        <v>0.7990229613149598</v>
+        <v>0.7990229613149596</v>
       </c>
       <c r="L168" t="n">
         <v>4.725378787878788</v>
@@ -66331,7 +66331,7 @@
         <v>0.8080267137096774</v>
       </c>
       <c r="K169" t="n">
-        <v>0.8451698019000483</v>
+        <v>0.8451698019000482</v>
       </c>
       <c r="L169" t="n">
         <v>7.333333333333333</v>
@@ -66717,7 +66717,7 @@
         <v>0.7040259576612903</v>
       </c>
       <c r="K170" t="n">
-        <v>0.7932917025722713</v>
+        <v>0.7932917025722716</v>
       </c>
       <c r="L170" t="n">
         <v>3.1553030303030303</v>

</xml_diff>